<commit_message>
Finished with the functional spec and project plan. small change to gantt-chart
</commit_message>
<xml_diff>
--- a/gantt-chart_exam.xlsx
+++ b/gantt-chart_exam.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8fda248c8888d899/front_end/exam/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8fda248c8888d899/front_end/exam/Noroff Exam 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="8_{92D11D94-7E0C-4D48-8505-F2B714C11C86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{58D88825-E723-7B4D-8719-ECF69D1F7302}"/>
+  <xr:revisionPtr revIDLastSave="194" documentId="8_{92D11D94-7E0C-4D48-8505-F2B714C11C86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E8F4E9DF-E481-8C49-BA29-52B22F97D006}"/>
   <bookViews>
-    <workbookView xWindow="20920" yWindow="1520" windowWidth="36740" windowHeight="19840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3840" yWindow="1440" windowWidth="36740" windowHeight="19840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -1096,9 +1096,6 @@
     <t>Days</t>
   </si>
   <si>
-    <t>Create a microsite for NASA/SpaceX</t>
-  </si>
-  <si>
     <t>Project Exam 1</t>
   </si>
   <si>
@@ -1153,10 +1150,13 @@
     <t>Deliver</t>
   </si>
   <si>
-    <t>Prototype</t>
-  </si>
-  <si>
     <t>Finalize</t>
+  </si>
+  <si>
+    <t>Create a microsite for SpaceX</t>
+  </si>
+  <si>
+    <t>Wireframe &amp; Prototype</t>
   </si>
 </sst>
 </file>
@@ -2225,6 +2225,13 @@
     <xf numFmtId="0" fontId="38" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="41" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2234,6 +2241,10 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="41" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="41" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2242,17 +2253,6 @@
     </xf>
     <xf numFmtId="167" fontId="41" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="41" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="41" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3088,8 +3088,8 @@
   <dimension ref="A1:CA48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3109,7 +3109,7 @@
   <sheetData>
     <row r="1" spans="1:79" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="78" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
@@ -3117,31 +3117,31 @@
       <c r="E1" s="43"/>
       <c r="F1" s="43"/>
       <c r="I1" s="82"/>
-      <c r="K1" s="123"/>
-      <c r="L1" s="123"/>
-      <c r="M1" s="123"/>
-      <c r="N1" s="123"/>
-      <c r="O1" s="123"/>
-      <c r="P1" s="123"/>
-      <c r="Q1" s="123"/>
-      <c r="R1" s="123"/>
-      <c r="S1" s="123"/>
-      <c r="T1" s="123"/>
-      <c r="U1" s="123"/>
-      <c r="V1" s="123"/>
-      <c r="W1" s="123"/>
-      <c r="X1" s="123"/>
-      <c r="Y1" s="123"/>
-      <c r="Z1" s="123"/>
-      <c r="AA1" s="123"/>
-      <c r="AB1" s="123"/>
-      <c r="AC1" s="123"/>
-      <c r="AD1" s="123"/>
-      <c r="AE1" s="123"/>
+      <c r="K1" s="117"/>
+      <c r="L1" s="117"/>
+      <c r="M1" s="117"/>
+      <c r="N1" s="117"/>
+      <c r="O1" s="117"/>
+      <c r="P1" s="117"/>
+      <c r="Q1" s="117"/>
+      <c r="R1" s="117"/>
+      <c r="S1" s="117"/>
+      <c r="T1" s="117"/>
+      <c r="U1" s="117"/>
+      <c r="V1" s="117"/>
+      <c r="W1" s="117"/>
+      <c r="X1" s="117"/>
+      <c r="Y1" s="117"/>
+      <c r="Z1" s="117"/>
+      <c r="AA1" s="117"/>
+      <c r="AB1" s="117"/>
+      <c r="AC1" s="117"/>
+      <c r="AD1" s="117"/>
+      <c r="AE1" s="117"/>
     </row>
     <row r="2" spans="1:79" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="48" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -3182,11 +3182,11 @@
       <c r="B4" s="76" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="125">
+      <c r="C4" s="122">
         <v>43941</v>
       </c>
-      <c r="D4" s="125"/>
-      <c r="E4" s="125"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
       <c r="F4" s="73"/>
       <c r="G4" s="76" t="s">
         <v>60</v>
@@ -3196,182 +3196,182 @@
       </c>
       <c r="I4" s="74"/>
       <c r="J4" s="46"/>
-      <c r="K4" s="117" t="str">
+      <c r="K4" s="119" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="118"/>
-      <c r="M4" s="118"/>
-      <c r="N4" s="118"/>
-      <c r="O4" s="118"/>
-      <c r="P4" s="118"/>
-      <c r="Q4" s="119"/>
-      <c r="R4" s="117" t="str">
+      <c r="L4" s="120"/>
+      <c r="M4" s="120"/>
+      <c r="N4" s="120"/>
+      <c r="O4" s="120"/>
+      <c r="P4" s="120"/>
+      <c r="Q4" s="121"/>
+      <c r="R4" s="119" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="118"/>
-      <c r="T4" s="118"/>
-      <c r="U4" s="118"/>
-      <c r="V4" s="118"/>
-      <c r="W4" s="118"/>
-      <c r="X4" s="119"/>
-      <c r="Y4" s="117" t="str">
+      <c r="S4" s="120"/>
+      <c r="T4" s="120"/>
+      <c r="U4" s="120"/>
+      <c r="V4" s="120"/>
+      <c r="W4" s="120"/>
+      <c r="X4" s="121"/>
+      <c r="Y4" s="119" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="118"/>
-      <c r="AA4" s="118"/>
-      <c r="AB4" s="118"/>
-      <c r="AC4" s="118"/>
-      <c r="AD4" s="118"/>
-      <c r="AE4" s="119"/>
-      <c r="AF4" s="117" t="str">
+      <c r="Z4" s="120"/>
+      <c r="AA4" s="120"/>
+      <c r="AB4" s="120"/>
+      <c r="AC4" s="120"/>
+      <c r="AD4" s="120"/>
+      <c r="AE4" s="121"/>
+      <c r="AF4" s="119" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="118"/>
-      <c r="AH4" s="118"/>
-      <c r="AI4" s="118"/>
-      <c r="AJ4" s="118"/>
-      <c r="AK4" s="118"/>
-      <c r="AL4" s="119"/>
-      <c r="AM4" s="117" t="str">
+      <c r="AG4" s="120"/>
+      <c r="AH4" s="120"/>
+      <c r="AI4" s="120"/>
+      <c r="AJ4" s="120"/>
+      <c r="AK4" s="120"/>
+      <c r="AL4" s="121"/>
+      <c r="AM4" s="119" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="118"/>
-      <c r="AO4" s="118"/>
-      <c r="AP4" s="118"/>
-      <c r="AQ4" s="118"/>
-      <c r="AR4" s="118"/>
-      <c r="AS4" s="119"/>
-      <c r="AT4" s="117" t="str">
+      <c r="AN4" s="120"/>
+      <c r="AO4" s="120"/>
+      <c r="AP4" s="120"/>
+      <c r="AQ4" s="120"/>
+      <c r="AR4" s="120"/>
+      <c r="AS4" s="121"/>
+      <c r="AT4" s="119" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="118"/>
-      <c r="AV4" s="118"/>
-      <c r="AW4" s="118"/>
-      <c r="AX4" s="118"/>
-      <c r="AY4" s="118"/>
-      <c r="AZ4" s="119"/>
-      <c r="BA4" s="117" t="str">
+      <c r="AU4" s="120"/>
+      <c r="AV4" s="120"/>
+      <c r="AW4" s="120"/>
+      <c r="AX4" s="120"/>
+      <c r="AY4" s="120"/>
+      <c r="AZ4" s="121"/>
+      <c r="BA4" s="119" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="118"/>
-      <c r="BC4" s="118"/>
-      <c r="BD4" s="118"/>
-      <c r="BE4" s="118"/>
-      <c r="BF4" s="118"/>
-      <c r="BG4" s="119"/>
-      <c r="BH4" s="117" t="str">
+      <c r="BB4" s="120"/>
+      <c r="BC4" s="120"/>
+      <c r="BD4" s="120"/>
+      <c r="BE4" s="120"/>
+      <c r="BF4" s="120"/>
+      <c r="BG4" s="121"/>
+      <c r="BH4" s="119" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="118"/>
-      <c r="BJ4" s="118"/>
-      <c r="BK4" s="118"/>
-      <c r="BL4" s="118"/>
-      <c r="BM4" s="118"/>
-      <c r="BN4" s="119"/>
+      <c r="BI4" s="120"/>
+      <c r="BJ4" s="120"/>
+      <c r="BK4" s="120"/>
+      <c r="BL4" s="120"/>
+      <c r="BM4" s="120"/>
+      <c r="BN4" s="121"/>
     </row>
     <row r="5" spans="1:79" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="72"/>
       <c r="B5" s="76" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="124" t="s">
+      <c r="C5" s="118" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="124"/>
-      <c r="E5" s="124"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
       <c r="F5" s="75"/>
       <c r="G5" s="75"/>
       <c r="H5" s="75"/>
       <c r="I5" s="75"/>
       <c r="J5" s="46"/>
-      <c r="K5" s="120">
+      <c r="K5" s="123">
         <f>K6</f>
         <v>43941</v>
       </c>
-      <c r="L5" s="121"/>
-      <c r="M5" s="121"/>
-      <c r="N5" s="121"/>
-      <c r="O5" s="121"/>
-      <c r="P5" s="121"/>
-      <c r="Q5" s="122"/>
-      <c r="R5" s="120">
+      <c r="L5" s="124"/>
+      <c r="M5" s="124"/>
+      <c r="N5" s="124"/>
+      <c r="O5" s="124"/>
+      <c r="P5" s="124"/>
+      <c r="Q5" s="125"/>
+      <c r="R5" s="123">
         <f>R6</f>
         <v>43948</v>
       </c>
-      <c r="S5" s="121"/>
-      <c r="T5" s="121"/>
-      <c r="U5" s="121"/>
-      <c r="V5" s="121"/>
-      <c r="W5" s="121"/>
-      <c r="X5" s="122"/>
-      <c r="Y5" s="120">
+      <c r="S5" s="124"/>
+      <c r="T5" s="124"/>
+      <c r="U5" s="124"/>
+      <c r="V5" s="124"/>
+      <c r="W5" s="124"/>
+      <c r="X5" s="125"/>
+      <c r="Y5" s="123">
         <f>Y6</f>
         <v>43955</v>
       </c>
-      <c r="Z5" s="121"/>
-      <c r="AA5" s="121"/>
-      <c r="AB5" s="121"/>
-      <c r="AC5" s="121"/>
-      <c r="AD5" s="121"/>
-      <c r="AE5" s="122"/>
-      <c r="AF5" s="120">
+      <c r="Z5" s="124"/>
+      <c r="AA5" s="124"/>
+      <c r="AB5" s="124"/>
+      <c r="AC5" s="124"/>
+      <c r="AD5" s="124"/>
+      <c r="AE5" s="125"/>
+      <c r="AF5" s="123">
         <f>AF6</f>
         <v>43962</v>
       </c>
-      <c r="AG5" s="121"/>
-      <c r="AH5" s="121"/>
-      <c r="AI5" s="121"/>
-      <c r="AJ5" s="121"/>
-      <c r="AK5" s="121"/>
-      <c r="AL5" s="122"/>
-      <c r="AM5" s="120">
+      <c r="AG5" s="124"/>
+      <c r="AH5" s="124"/>
+      <c r="AI5" s="124"/>
+      <c r="AJ5" s="124"/>
+      <c r="AK5" s="124"/>
+      <c r="AL5" s="125"/>
+      <c r="AM5" s="123">
         <f>AM6</f>
         <v>43969</v>
       </c>
-      <c r="AN5" s="121"/>
-      <c r="AO5" s="121"/>
-      <c r="AP5" s="121"/>
-      <c r="AQ5" s="121"/>
-      <c r="AR5" s="121"/>
-      <c r="AS5" s="122"/>
-      <c r="AT5" s="120">
+      <c r="AN5" s="124"/>
+      <c r="AO5" s="124"/>
+      <c r="AP5" s="124"/>
+      <c r="AQ5" s="124"/>
+      <c r="AR5" s="124"/>
+      <c r="AS5" s="125"/>
+      <c r="AT5" s="123">
         <f>AT6</f>
         <v>43976</v>
       </c>
-      <c r="AU5" s="121"/>
-      <c r="AV5" s="121"/>
-      <c r="AW5" s="121"/>
-      <c r="AX5" s="121"/>
-      <c r="AY5" s="121"/>
-      <c r="AZ5" s="122"/>
-      <c r="BA5" s="120">
+      <c r="AU5" s="124"/>
+      <c r="AV5" s="124"/>
+      <c r="AW5" s="124"/>
+      <c r="AX5" s="124"/>
+      <c r="AY5" s="124"/>
+      <c r="AZ5" s="125"/>
+      <c r="BA5" s="123">
         <f>BA6</f>
         <v>43983</v>
       </c>
-      <c r="BB5" s="121"/>
-      <c r="BC5" s="121"/>
-      <c r="BD5" s="121"/>
-      <c r="BE5" s="121"/>
-      <c r="BF5" s="121"/>
-      <c r="BG5" s="122"/>
-      <c r="BH5" s="120">
+      <c r="BB5" s="124"/>
+      <c r="BC5" s="124"/>
+      <c r="BD5" s="124"/>
+      <c r="BE5" s="124"/>
+      <c r="BF5" s="124"/>
+      <c r="BG5" s="125"/>
+      <c r="BH5" s="123">
         <f>BH6</f>
         <v>43990</v>
       </c>
-      <c r="BI5" s="121"/>
-      <c r="BJ5" s="121"/>
-      <c r="BK5" s="121"/>
-      <c r="BL5" s="121"/>
-      <c r="BM5" s="121"/>
-      <c r="BN5" s="122"/>
+      <c r="BI5" s="124"/>
+      <c r="BJ5" s="124"/>
+      <c r="BK5" s="124"/>
+      <c r="BL5" s="124"/>
+      <c r="BM5" s="124"/>
+      <c r="BN5" s="125"/>
     </row>
     <row r="6" spans="1:79" x14ac:dyDescent="0.15">
       <c r="A6" s="45"/>
@@ -3700,7 +3700,7 @@
         <v>1.1</v>
       </c>
       <c r="B8" s="79" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D8" s="80"/>
       <c r="E8" s="67">
@@ -3779,7 +3779,7 @@
         <v>1.2</v>
       </c>
       <c r="B9" s="79" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D9" s="80"/>
       <c r="E9" s="67">
@@ -3858,7 +3858,7 @@
         <v>1.3</v>
       </c>
       <c r="B10" s="79" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D10" s="80"/>
       <c r="E10" s="67">
@@ -3937,7 +3937,7 @@
         <v>1.4</v>
       </c>
       <c r="B11" s="79" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D11" s="80"/>
       <c r="E11" s="67">
@@ -4016,7 +4016,7 @@
         <v>1.5</v>
       </c>
       <c r="B12" s="79" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D12" s="80"/>
       <c r="E12" s="67">
@@ -4095,7 +4095,7 @@
         <v>1.6</v>
       </c>
       <c r="B13" s="79" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D13" s="80"/>
       <c r="E13" s="67">
@@ -4174,7 +4174,7 @@
         <v>1.7</v>
       </c>
       <c r="B14" s="79" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D14" s="80"/>
       <c r="E14" s="67">
@@ -4624,7 +4624,7 @@
         <v>2.1</v>
       </c>
       <c r="B19" s="79" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C19" s="51"/>
       <c r="D19" s="80"/>
@@ -4717,7 +4717,7 @@
         <v>2.2</v>
       </c>
       <c r="B20" s="79" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C20" s="51"/>
       <c r="D20" s="80"/>
@@ -4810,7 +4810,7 @@
         <v>2.3</v>
       </c>
       <c r="B21" s="79" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C21" s="51"/>
       <c r="D21" s="80"/>
@@ -4903,7 +4903,7 @@
         <v>2.4</v>
       </c>
       <c r="B22" s="79" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C22" s="51"/>
       <c r="D22" s="80"/>
@@ -4996,7 +4996,7 @@
         <v>2.5</v>
       </c>
       <c r="B23" s="79" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C23" s="51"/>
       <c r="D23" s="80"/>
@@ -5367,7 +5367,7 @@
         <v>3.1</v>
       </c>
       <c r="B27" s="79" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C27" s="51"/>
       <c r="D27" s="80"/>
@@ -5460,7 +5460,7 @@
         <v>3.2</v>
       </c>
       <c r="B28" s="79" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C28" s="51"/>
       <c r="D28" s="80"/>
@@ -5553,7 +5553,7 @@
         <v>3.3</v>
       </c>
       <c r="B29" s="79" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C29" s="51"/>
       <c r="D29" s="80"/>
@@ -5646,7 +5646,7 @@
         <v>3.4</v>
       </c>
       <c r="B30" s="79" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C30" s="51"/>
       <c r="D30" s="80"/>
@@ -6017,7 +6017,7 @@
         <v>4.1</v>
       </c>
       <c r="B34" s="79" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C34" s="51"/>
       <c r="D34" s="80"/>
@@ -6110,7 +6110,7 @@
         <v>4.2</v>
       </c>
       <c r="B35" s="79" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C35" s="51"/>
       <c r="D35" s="80"/>
@@ -6203,7 +6203,7 @@
         <v>4.3</v>
       </c>
       <c r="B36" s="79" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C36" s="51"/>
       <c r="D36" s="80"/>
@@ -6296,7 +6296,7 @@
         <v>4.4</v>
       </c>
       <c r="B37" s="79" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C37" s="51"/>
       <c r="D37" s="80"/>
@@ -6760,7 +6760,7 @@
         <v>5.1</v>
       </c>
       <c r="B42" s="79" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C42" s="51"/>
       <c r="D42" s="80"/>
@@ -6853,7 +6853,7 @@
         <v>5.2</v>
       </c>
       <c r="B43" s="79" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C43" s="51"/>
       <c r="D43" s="80"/>
@@ -6946,7 +6946,7 @@
         <v>5.3</v>
       </c>
       <c r="B44" s="79" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C44" s="51"/>
       <c r="D44" s="80"/>
@@ -7039,7 +7039,7 @@
         <v>5.4</v>
       </c>
       <c r="B45" s="79" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C45" s="51"/>
       <c r="D45" s="80"/>
@@ -7408,15 +7408,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -7427,6 +7418,15 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H7:H48">

</xml_diff>